<commit_message>
Update Sprint 3 Burndown Chart Version 1.xlsx
</commit_message>
<xml_diff>
--- a/_sprints/sprint3/burndown/Sprint 3 Burndown Chart Version 1.xlsx
+++ b/_sprints/sprint3/burndown/Sprint 3 Burndown Chart Version 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Grad School\Emerging Processes\adventra-app\_sprints\sprint3\burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F5FAA2-D691-4D02-AACD-AAACB84E9118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84081C02-08B9-4792-B3C8-C73F140451A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1185" windowWidth="21600" windowHeight="11295" xr2:uid="{5E7660C9-43B9-406B-90F3-620F8B00C16F}"/>
   </bookViews>
@@ -307,7 +307,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1625,7 +1625,7 @@
   <dimension ref="C6:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
         <v>9</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>

</xml_diff>